<commit_message>
Made changes to the data model values to fit the data and also added Decision_Tress.py and updated the fake_data.xlsx and values of Engineering_data.xlsx
</commit_message>
<xml_diff>
--- a/Engineering_data.xlsx
+++ b/Engineering_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nitin\PycharmProjects\ML_Stator_Hairline_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90F7D554-1E59-42A6-A48E-B25DD272A41D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFD76EB-6280-4EC4-A8AB-3C8CB023457D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6576" yWindow="3504" windowWidth="17280" windowHeight="8880" xr2:uid="{0074EBF8-F3D6-4585-8A8E-7B53F138148F}"/>
+    <workbookView xWindow="4764" yWindow="2940" windowWidth="17280" windowHeight="8880" xr2:uid="{0074EBF8-F3D6-4585-8A8E-7B53F138148F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,13 +530,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>38.5</v>
+        <v>28.5</v>
       </c>
       <c r="D4">
-        <v>41.5</v>
+        <v>31.5</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>